<commit_message>
add additional Hucuktlis age samples
</commit_message>
<xml_diff>
--- a/1. data/return by age time series.xlsx
+++ b/1. data/return by age time series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB61B266-A4A9-4416-8D3D-E20920168B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D11B4A1-9F96-4C56-BDA3-0D33DB2AB917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="15375" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Somass" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="37">
   <si>
     <t>GCL</t>
   </si>
@@ -11809,10 +11809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A94BF84-AB01-45F2-8A1E-DD5B502642C6}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13700,6 +13700,30 @@
       <c r="D57" t="s">
         <v>34</v>
       </c>
+      <c r="E57">
+        <v>16</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -13714,6 +13738,9 @@
       <c r="D58" t="s">
         <v>34</v>
       </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -13793,40 +13820,116 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
+        <v>2022</v>
+      </c>
+      <c r="B61">
+        <v>18646</v>
+      </c>
+      <c r="C61">
+        <v>7731</v>
+      </c>
+      <c r="D61" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61">
+        <v>15</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H61">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>2023</v>
       </c>
-      <c r="B61">
+      <c r="B62">
         <v>13113</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>8196</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>36</v>
       </c>
-      <c r="E61">
+      <c r="E62">
         <v>151</v>
       </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
         <v>0.19867549668874171</v>
       </c>
-      <c r="H61">
+      <c r="H62">
         <v>0.7814569536423841</v>
       </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
         <v>6.6225165562913907E-3</v>
       </c>
-      <c r="L61">
+      <c r="L62">
         <v>1.3245033112582781E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2023</v>
+      </c>
+      <c r="B63">
+        <v>13113</v>
+      </c>
+      <c r="C63">
+        <v>8196</v>
+      </c>
+      <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63">
+        <v>7</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="H63">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>